<commit_message>
Append additional info to the start file
</commit_message>
<xml_diff>
--- a/start_bestand.xlsx
+++ b/start_bestand.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nordendeu-my.sharepoint.com/personal/dries_nordend_eu/Documents/projects/AWV/python_repositories/OTLMOW-PostenMapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_CB51155F1056087EEC42C41548B8B6FF58B3D7D8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D15B6D80-223F-42D6-9643-A1BBFB8731E4}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="11_CB51155F1056087EEC42C41548B8B6FF58B3D7D8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CA97207-D3E2-49B4-81F9-E9EE1B4C10AD}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="onderdeel#WVLichtmast" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>typeURI</t>
   </si>
@@ -71,6 +71,24 @@
   </si>
   <si>
     <t>dummyNaam5</t>
+  </si>
+  <si>
+    <t>heeftStopcontact</t>
+  </si>
+  <si>
+    <t>masthoogte.standaardHoogte</t>
+  </si>
+  <si>
+    <t>10.00</t>
+  </si>
+  <si>
+    <t>12.00</t>
+  </si>
+  <si>
+    <t>18.00</t>
+  </si>
+  <si>
+    <t>20.00</t>
   </si>
 </sst>
 </file>
@@ -416,18 +434,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,8 +463,14 @@
       <c r="E1" t="s">
         <v>11</v>
       </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -457,8 +483,11 @@
       <c r="E2" t="s">
         <v>12</v>
       </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -471,8 +500,11 @@
       <c r="E3" t="s">
         <v>13</v>
       </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -485,8 +517,14 @@
       <c r="E4" t="s">
         <v>14</v>
       </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -499,8 +537,14 @@
       <c r="E5" t="s">
         <v>15</v>
       </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -512,6 +556,9 @@
       </c>
       <c r="E6" t="s">
         <v>16</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>